<commit_message>
Bug fixes and new penalty
Signed-off-by: Michael Billard <angel125@spellflight.com>
</commit_message>
<xml_diff>
--- a/GameData/Snacks/Docs/Snacks Trip Planner.xlsx
+++ b/GameData/Snacks/Docs/Snacks Trip Planner.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\KSP\Snacks\GameData\Snacks\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KSPDev\GameData\Snacks\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
   <si>
     <t>Water</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Resources Consumed</t>
   </si>
   <si>
-    <t>unis</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -222,12 +219,18 @@
   </si>
   <si>
     <t>* System is calibrated to these numbers as standard</t>
+  </si>
+  <si>
+    <t>Required Resources</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -274,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -282,6 +285,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,9 +566,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -572,6 +576,7 @@
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -594,7 +599,6 @@
         <v>32</v>
       </c>
       <c r="B2">
-        <f>G27</f>
         <v>28</v>
       </c>
       <c r="C2" t="s">
@@ -641,7 +645,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -668,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -680,7 +684,7 @@
         <v>25</v>
       </c>
       <c r="M5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N5">
         <v>1E-3</v>
@@ -736,10 +740,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1">
-        <f>G27*(B4*B5*B3)</f>
+        <f>B2*(B4*B5*B3)</f>
         <v>168</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -759,7 +763,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1">
         <f>B8</f>
@@ -781,7 +785,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>39</v>
@@ -822,7 +826,7 @@
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -844,7 +848,7 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -868,8 +872,9 @@
       <c r="F15" t="s">
         <v>0</v>
       </c>
-      <c r="G15">
-        <v>5.0000000000000002E-5</v>
+      <c r="G15" s="5">
+        <f>G17/4</f>
+        <v>6.9444444444444444E-5</v>
       </c>
       <c r="H15" t="s">
         <v>48</v>
@@ -894,10 +899,11 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16">
-        <v>5.0000000000000002E-5</v>
+        <v>57</v>
+      </c>
+      <c r="G16" s="5">
+        <f>G17/4</f>
+        <v>6.9444444444444444E-5</v>
       </c>
       <c r="H16" t="s">
         <v>48</v>
@@ -910,8 +916,9 @@
       <c r="F17" t="s">
         <v>1</v>
       </c>
-      <c r="G17">
-        <v>2.7777999999999999E-4</v>
+      <c r="G17" s="5">
+        <f>B7/21600</f>
+        <v>2.7777777777777778E-4</v>
       </c>
       <c r="H17" t="s">
         <v>48</v>
@@ -956,7 +963,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="3">
         <v>200</v>
@@ -968,11 +975,11 @@
       </c>
       <c r="G21">
         <f>G15*21600</f>
-        <v>1.08</v>
+        <v>1.5</v>
       </c>
       <c r="H21">
         <f>G21*N2</f>
-        <v>1.08E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="I21" t="s">
         <v>29</v>
@@ -987,16 +994,16 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="F22" t="s">
-        <v>1</v>
+      <c r="F22" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="G22">
-        <f>G17*21600</f>
-        <v>6.0000479999999996</v>
+        <f>G16*21600</f>
+        <v>1.5</v>
       </c>
       <c r="H22">
-        <f>G22*N3</f>
-        <v>6.000048E-3</v>
+        <f>G22*N5</f>
+        <v>1.5E-3</v>
       </c>
       <c r="I22" t="s">
         <v>29</v>
@@ -1012,16 +1019,16 @@
       <c r="D23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>58</v>
+      <c r="F23" t="s">
+        <v>1</v>
       </c>
       <c r="G23">
-        <f>G16*21600</f>
-        <v>1.08</v>
+        <f>G17*21600</f>
+        <v>6</v>
       </c>
       <c r="H23">
-        <f>G23*N5</f>
-        <v>1.08E-3</v>
+        <f>G23*N3</f>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="I23" t="s">
         <v>29</v>
@@ -1051,7 +1058,7 @@
       </c>
       <c r="H24">
         <f>SUM(H21:H23)</f>
-        <v>8.1600479999999996E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="I24" t="s">
         <v>45</v>
@@ -1093,6 +1100,7 @@
         <v>52</v>
       </c>
       <c r="G27">
+        <f>B2</f>
         <v>28</v>
       </c>
     </row>
@@ -1126,7 +1134,7 @@
         <v>9</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1147,13 +1155,13 @@
         <v>7</v>
       </c>
       <c r="G30">
-        <f>G22*G27</f>
-        <v>168.00134399999999</v>
+        <f>G23*G27</f>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31">
         <f>B8*N4</f>
@@ -1167,7 +1175,7 @@
       </c>
       <c r="G31">
         <f>G30*N4</f>
-        <v>0.168001344</v>
+        <v>0.16800000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1189,7 +1197,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="H34" t="s">
         <v>45</v>
@@ -1201,46 +1209,63 @@
       </c>
       <c r="G35">
         <f>G21*G27</f>
-        <v>30.240000000000002</v>
+        <v>42</v>
       </c>
       <c r="H35">
         <f>G35*N2</f>
-        <v>3.0240000000000003E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="G36">
         <f>G22*G27</f>
-        <v>168.00134399999999</v>
+        <v>42</v>
       </c>
       <c r="H36">
-        <f>G36*N3</f>
-        <v>0.168001344</v>
+        <f>G36*N5</f>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <f>G23*G27</f>
-        <v>30.240000000000002</v>
+        <v>168</v>
       </c>
       <c r="H37">
-        <f>G37*N5</f>
-        <v>3.0240000000000003E-2</v>
+        <f>G37*N3</f>
+        <v>0.16800000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H38">
         <f>SUM(H35:H37)</f>
-        <v>0.22848134399999998</v>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41">
+        <f>G35/2</f>
+        <v>21</v>
+      </c>
+      <c r="H41" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>